<commit_message>
Update Námskeið verkfræðideildar haustönn 2022 með undanförum.xlsx
</commit_message>
<xml_diff>
--- a/Námskeið verkfræðideildar haustönn 2022 með undanförum.xlsx
+++ b/Námskeið verkfræðideildar haustönn 2022 með undanförum.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/karitasetnaelmarsdottir/Documents/GitHub/LIKX2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5563838-2CB5-6D44-9201-1A432CE2E7A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26B3D3A2-46C9-5948-872B-75FE19CF83C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1272" uniqueCount="429">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1284" uniqueCount="429">
   <si>
     <t>CourseCode</t>
   </si>
@@ -1725,8 +1725,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M59"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="E54" sqref="E54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2122,6 +2122,9 @@
       <c r="D10" t="s">
         <v>15</v>
       </c>
+      <c r="E10" t="s">
+        <v>427</v>
+      </c>
       <c r="F10">
         <v>6</v>
       </c>
@@ -2160,6 +2163,9 @@
       <c r="D11" t="s">
         <v>15</v>
       </c>
+      <c r="E11" t="s">
+        <v>427</v>
+      </c>
       <c r="F11">
         <v>6</v>
       </c>
@@ -2198,6 +2204,9 @@
       <c r="D12" t="s">
         <v>15</v>
       </c>
+      <c r="E12" t="s">
+        <v>427</v>
+      </c>
       <c r="F12">
         <v>6</v>
       </c>
@@ -2274,6 +2283,9 @@
       <c r="D14" t="s">
         <v>15</v>
       </c>
+      <c r="E14" t="s">
+        <v>427</v>
+      </c>
       <c r="F14">
         <v>6</v>
       </c>
@@ -2350,6 +2362,9 @@
       <c r="D16" t="s">
         <v>15</v>
       </c>
+      <c r="E16" t="s">
+        <v>427</v>
+      </c>
       <c r="F16">
         <v>6</v>
       </c>
@@ -2426,6 +2441,9 @@
       <c r="D18" t="s">
         <v>15</v>
       </c>
+      <c r="E18" t="s">
+        <v>428</v>
+      </c>
       <c r="F18">
         <v>6</v>
       </c>
@@ -2464,6 +2482,9 @@
       <c r="D19" t="s">
         <v>15</v>
       </c>
+      <c r="E19" t="s">
+        <v>427</v>
+      </c>
       <c r="F19">
         <v>6</v>
       </c>
@@ -2540,6 +2561,9 @@
       <c r="D21" t="s">
         <v>15</v>
       </c>
+      <c r="E21" t="s">
+        <v>427</v>
+      </c>
       <c r="F21">
         <v>6</v>
       </c>
@@ -2578,6 +2602,9 @@
       <c r="D22" t="s">
         <v>15</v>
       </c>
+      <c r="E22" t="s">
+        <v>427</v>
+      </c>
       <c r="F22">
         <v>6</v>
       </c>
@@ -2616,6 +2643,9 @@
       <c r="D23" t="s">
         <v>15</v>
       </c>
+      <c r="E23" t="s">
+        <v>428</v>
+      </c>
       <c r="F23">
         <v>6</v>
       </c>
@@ -2806,6 +2836,9 @@
       <c r="D28" t="s">
         <v>15</v>
       </c>
+      <c r="E28" t="s">
+        <v>427</v>
+      </c>
       <c r="F28">
         <v>6</v>
       </c>
@@ -2843,6 +2876,9 @@
       </c>
       <c r="D29" t="s">
         <v>15</v>
+      </c>
+      <c r="E29" t="s">
+        <v>427</v>
       </c>
       <c r="F29">
         <v>6</v>

</xml_diff>